<commit_message>
Initial - 23 Sep 2024
</commit_message>
<xml_diff>
--- a/TestData/TMTC0032668_VerifyActivityIsLinkedToTheRelatedCampaign.xlsx
+++ b/TestData/TMTC0032668_VerifyActivityIsLinkedToTheRelatedCampaign.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMittal0207\source\repos\SF_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D51843D-3136-492E-8B7B-58A6972F3C3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C3EBB2D-3838-471F-875E-0DBA18742C2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="2" r:id="rId1"/>
     <sheet name="Contact" sheetId="10" r:id="rId2"/>
     <sheet name="Activity" sheetId="11" r:id="rId3"/>
+    <sheet name="Campaign" sheetId="12" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Users</t>
   </si>
@@ -110,6 +111,12 @@
   </si>
   <si>
     <t>OpportunityCFTest</t>
+  </si>
+  <si>
+    <t>RecordType</t>
+  </si>
+  <si>
+    <t>Parent Campaign</t>
   </si>
 </sst>
 </file>
@@ -518,7 +525,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DB9990D-2177-413E-8716-FEF5A04433C7}">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
@@ -591,4 +598,30 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F88B6D4-1355-429D-BB94-34D3365E64A7}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="14.88671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Mid - TMT0072236_VerifyActivityIsLinkedToTheRelatedCampaign - 23 Sep 2024
</commit_message>
<xml_diff>
--- a/TestData/TMTC0032668_VerifyActivityIsLinkedToTheRelatedCampaign.xlsx
+++ b/TestData/TMTC0032668_VerifyActivityIsLinkedToTheRelatedCampaign.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMittal0207\source\repos\SF_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C3EBB2D-3838-471F-875E-0DBA18742C2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CB0327A-EB2B-4423-ABDD-857280A96CC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="2" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="35">
   <si>
     <t>Users</t>
   </si>
@@ -117,6 +117,33 @@
   </si>
   <si>
     <t>Parent Campaign</t>
+  </si>
+  <si>
+    <t>CampaignName</t>
+  </si>
+  <si>
+    <t>TestParentCampaign</t>
+  </si>
+  <si>
+    <t>LOB</t>
+  </si>
+  <si>
+    <t>CF</t>
+  </si>
+  <si>
+    <t>IndustryGroups</t>
+  </si>
+  <si>
+    <t>BUS</t>
+  </si>
+  <si>
+    <t>HLSubGroup</t>
+  </si>
+  <si>
+    <t>CM</t>
+  </si>
+  <si>
+    <t>Campaigns</t>
   </si>
 </sst>
 </file>
@@ -523,10 +550,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DB9990D-2177-413E-8716-FEF5A04433C7}">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -539,9 +566,10 @@
     <col min="6" max="6" width="14.5546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="19.5546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="20.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -566,8 +594,11 @@
       <c r="H1" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I1" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -591,6 +622,9 @@
       </c>
       <c r="H2" t="s">
         <v>23</v>
+      </c>
+      <c r="I2" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -602,23 +636,51 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F88B6D4-1355-429D-BB94-34D3365E64A7}">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>25</v>
+      </c>
+      <c r="B2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E2" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
TMT0072236_VerifyActivityIsLinkedToTheRelatedCampaign - Final - 23 Sep 2024
</commit_message>
<xml_diff>
--- a/TestData/TMTC0032668_VerifyActivityIsLinkedToTheRelatedCampaign.xlsx
+++ b/TestData/TMTC0032668_VerifyActivityIsLinkedToTheRelatedCampaign.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMittal0207\source\repos\SF_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CB0327A-EB2B-4423-ABDD-857280A96CC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64C3EB1A-8B7A-476F-A23D-CD4EA28C82AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -95,12 +95,6 @@
     <t>Activity Test External Contact</t>
   </si>
   <si>
-    <t>Company Discussed Meeting</t>
-  </si>
-  <si>
-    <t>Company Discussed Meeting Description</t>
-  </si>
-  <si>
     <t>CompanyDiscussed</t>
   </si>
   <si>
@@ -144,6 +138,12 @@
   </si>
   <si>
     <t>Campaigns</t>
+  </si>
+  <si>
+    <t>Related Campaign Meeting</t>
+  </si>
+  <si>
+    <t>Related Campaign Meeting Description</t>
   </si>
 </sst>
 </file>
@@ -553,7 +553,7 @@
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -589,13 +589,13 @@
         <v>6</v>
       </c>
       <c r="G1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="H1" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="I1" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
@@ -603,7 +603,7 @@
         <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>18</v>
+        <v>33</v>
       </c>
       <c r="C2" t="s">
         <v>8</v>
@@ -612,19 +612,19 @@
         <v>9</v>
       </c>
       <c r="E2" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="F2" t="s">
         <v>12</v>
       </c>
       <c r="G2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H2" t="s">
         <v>21</v>
       </c>
-      <c r="H2" t="s">
-        <v>23</v>
-      </c>
       <c r="I2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -651,36 +651,36 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" t="s">
         <v>25</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>27</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>29</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>31</v>
-      </c>
-      <c r="E2" t="s">
-        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Activities & Contacts changes - 16 Apr 2025
</commit_message>
<xml_diff>
--- a/TestData/TMTC0032668_VerifyActivityIsLinkedToTheRelatedCampaign.xlsx
+++ b/TestData/TMTC0032668_VerifyActivityIsLinkedToTheRelatedCampaign.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMittal0207\source\repos\SF_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64C3EB1A-8B7A-476F-A23D-CD4EA28C82AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB3BEEA4-9DB2-4A73-9207-9167508B53E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3624" yWindow="1500" windowWidth="19416" windowHeight="10740" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="2" r:id="rId1"/>
@@ -134,9 +134,6 @@
     <t>HLSubGroup</t>
   </si>
   <si>
-    <t>CM</t>
-  </si>
-  <si>
     <t>Campaigns</t>
   </si>
   <si>
@@ -144,6 +141,9 @@
   </si>
   <si>
     <t>Related Campaign Meeting Description</t>
+  </si>
+  <si>
+    <t>BAS</t>
   </si>
 </sst>
 </file>
@@ -552,7 +552,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DB9990D-2177-413E-8716-FEF5A04433C7}">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
@@ -595,7 +595,7 @@
         <v>20</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
@@ -603,7 +603,7 @@
         <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C2" t="s">
         <v>8</v>
@@ -612,7 +612,7 @@
         <v>9</v>
       </c>
       <c r="E2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F2" t="s">
         <v>12</v>
@@ -638,7 +638,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F88B6D4-1355-429D-BB94-34D3365E64A7}">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
@@ -680,7 +680,7 @@
         <v>29</v>
       </c>
       <c r="E2" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Test Data update - 8th July 2025
</commit_message>
<xml_diff>
--- a/TestData/TMTC0032668_VerifyActivityIsLinkedToTheRelatedCampaign.xlsx
+++ b/TestData/TMTC0032668_VerifyActivityIsLinkedToTheRelatedCampaign.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMittal0207\source\repos\SF_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB3BEEA4-9DB2-4A73-9207-9167508B53E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C330160-0C4E-4832-B7B3-1EFD1861A7EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3624" yWindow="1500" windowWidth="19416" windowHeight="10740" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="2" r:id="rId1"/>
@@ -143,7 +143,7 @@
     <t>Related Campaign Meeting Description</t>
   </si>
   <si>
-    <t>BAS</t>
+    <t>None</t>
   </si>
 </sst>
 </file>
@@ -485,17 +485,17 @@
       <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -514,13 +514,13 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
@@ -531,7 +531,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -556,20 +556,20 @@
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="33.21875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="33.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -598,7 +598,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -642,14 +642,14 @@
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>22</v>
       </c>
@@ -666,7 +666,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>23</v>
       </c>

</xml_diff>